<commit_message>
BackLog finalizado para Sprint1
</commit_message>
<xml_diff>
--- a/documentaçao/ProductBacklog.xlsx
+++ b/documentaçao/ProductBacklog.xlsx
@@ -1,17 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25108"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A25F24B9-8173-4BC5-A4A7-6604FB42FA61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="885"/>
   </bookViews>
   <sheets>
     <sheet name="PBC" sheetId="15" r:id="rId1"/>
     <sheet name="Dados" sheetId="14" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="64">
   <si>
     <t>Product BackLog Classified (PBC)</t>
   </si>
@@ -228,11 +227,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="18">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -319,6 +318,16 @@
       <name val="Barlow"/>
     </font>
     <font>
+      <sz val="12"/>
+      <name val="Barlow"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="14"/>
+      <name val="Barlow"/>
+    </font>
+    <font>
+      <u/>
       <sz val="12"/>
       <name val="Barlow"/>
     </font>
@@ -646,7 +655,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -761,9 +770,6 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -830,31 +836,364 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="21">
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="34">
+  <dxfs count="73">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FFEFB661"/>
+          <bgColor rgb="FFEFB661"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFC8D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FFEFB661"/>
+          <bgColor rgb="FFEFB661"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFC8D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFEFB661"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFC8D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FFEFB661"/>
+          <bgColor rgb="FFEFB661"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFC8D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FFEFB661"/>
+          <bgColor rgb="FFEFB661"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFC8D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FFEFB661"/>
+          <bgColor rgb="FFEFB661"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFC8D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FFEFB661"/>
+          <bgColor rgb="FFEFB661"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFC8D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FFEFB661"/>
+          <bgColor rgb="FFEFB661"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFC8D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1244,7 +1583,7 @@
         <xdr:cNvPr id="4" name="Imagem 3" descr="Logo SPTECH">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28E092BE-8680-4E85-8060-49F631E5D5E9}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28E092BE-8680-4E85-8060-49F631E5D5E9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1611,10 +1950,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H51"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
@@ -1633,72 +1972,61 @@
   <sheetData>
     <row r="1" spans="2:8" ht="17.25" customHeight="1" thickBot="1"/>
     <row r="2" spans="2:8" ht="89.25" customHeight="1" thickBot="1">
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="57"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="56"/>
       <c r="H2"/>
     </row>
     <row r="3" spans="2:8" ht="9.9499999999999993" customHeight="1" thickBot="1"/>
     <row r="4" spans="2:8" s="25" customFormat="1" ht="43.5" customHeight="1" thickBot="1">
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="41" t="s">
+      <c r="C4" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="43" t="s">
+      <c r="D4" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="44" t="s">
+      <c r="E4" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="45" t="s">
+      <c r="F4" s="44" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="2:8" s="26" customFormat="1" ht="23.1" customHeight="1">
-      <c r="B5" s="46">
+      <c r="C5" s="38"/>
+      <c r="F5" s="39"/>
+    </row>
+    <row r="6" spans="2:8" s="26" customFormat="1" ht="23.1" customHeight="1">
+      <c r="B6" s="45">
         <v>1</v>
-      </c>
-      <c r="C5" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="40"/>
-    </row>
-    <row r="6" spans="2:8" s="26" customFormat="1" ht="23.1" customHeight="1">
-      <c r="B6" s="27">
-        <v>2</v>
       </c>
       <c r="C6" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="53" t="s">
-        <v>9</v>
+      <c r="D6" s="51" t="s">
+        <v>16</v>
       </c>
       <c r="E6" s="29">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F6" s="32"/>
     </row>
     <row r="7" spans="2:8" s="26" customFormat="1" ht="23.1" customHeight="1">
-      <c r="B7" s="47">
-        <v>3</v>
+      <c r="B7" s="27">
+        <v>2</v>
       </c>
       <c r="C7" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="54" t="s">
-        <v>10</v>
+      <c r="D7" s="50" t="s">
+        <v>7</v>
       </c>
       <c r="E7" s="29">
         <v>5</v>
@@ -1706,14 +2034,14 @@
       <c r="F7" s="32"/>
     </row>
     <row r="8" spans="2:8" s="26" customFormat="1" ht="23.1" customHeight="1">
-      <c r="B8" s="27">
-        <v>4</v>
+      <c r="B8" s="46">
+        <v>3</v>
       </c>
       <c r="C8" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="52" t="s">
-        <v>11</v>
+      <c r="D8" s="53" t="s">
+        <v>10</v>
       </c>
       <c r="E8" s="29">
         <v>3</v>
@@ -1722,13 +2050,13 @@
     </row>
     <row r="9" spans="2:8" s="26" customFormat="1" ht="22.5" customHeight="1">
       <c r="B9" s="27">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C9" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="53" t="s">
-        <v>12</v>
+      <c r="D9" s="52" t="s">
+        <v>17</v>
       </c>
       <c r="E9" s="29">
         <v>8</v>
@@ -1737,103 +2065,103 @@
     </row>
     <row r="10" spans="2:8" s="26" customFormat="1" ht="23.1" customHeight="1">
       <c r="B10" s="27">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C10" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="52" t="s">
-        <v>13</v>
+      <c r="D10" s="51" t="s">
+        <v>11</v>
       </c>
       <c r="E10" s="29">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F10" s="32"/>
     </row>
     <row r="11" spans="2:8" s="26" customFormat="1" ht="23.1" customHeight="1">
       <c r="B11" s="27">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C11" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="52" t="s">
+      <c r="D11" s="51" t="s">
         <v>14</v>
       </c>
       <c r="E11" s="29">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F11" s="32"/>
     </row>
     <row r="12" spans="2:8" s="26" customFormat="1" ht="23.1" customHeight="1">
       <c r="B12" s="27">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C12" s="31" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="52" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E12" s="29">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F12" s="32"/>
     </row>
     <row r="13" spans="2:8" s="26" customFormat="1" ht="23.1" customHeight="1">
       <c r="B13" s="27">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C13" s="31" t="s">
         <v>6</v>
       </c>
       <c r="D13" s="52" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E13" s="29">
-        <v>3</v>
-      </c>
-      <c r="F13" s="32"/>
+        <v>5</v>
+      </c>
+      <c r="F13" s="60"/>
     </row>
     <row r="14" spans="2:8" s="26" customFormat="1" ht="23.1" customHeight="1">
       <c r="B14" s="27">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C14" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="53" t="s">
-        <v>17</v>
+      <c r="D14" s="51" t="s">
+        <v>15</v>
       </c>
       <c r="E14" s="29">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F14" s="32"/>
     </row>
     <row r="15" spans="2:8" s="26" customFormat="1" ht="23.1" customHeight="1">
       <c r="B15" s="27">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C15" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="28" t="s">
-        <v>18</v>
+      <c r="D15" s="51" t="s">
+        <v>13</v>
       </c>
       <c r="E15" s="29">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F15" s="32"/>
     </row>
     <row r="16" spans="2:8" s="26" customFormat="1" ht="23.1" customHeight="1">
       <c r="B16" s="27">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C16" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="28" t="s">
-        <v>19</v>
+      <c r="D16" s="59" t="s">
+        <v>18</v>
       </c>
       <c r="E16" s="29">
         <v>5</v>
@@ -1842,18 +2170,22 @@
     </row>
     <row r="17" spans="2:6" s="26" customFormat="1" ht="23.1" customHeight="1">
       <c r="B17" s="27">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C17" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="28"/>
-      <c r="E17" s="29"/>
+      <c r="D17" s="52" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="29">
+        <v>8</v>
+      </c>
       <c r="F17" s="32"/>
     </row>
     <row r="18" spans="2:6" s="26" customFormat="1" ht="23.1" customHeight="1">
       <c r="B18" s="27">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C18" s="31" t="s">
         <v>6</v>
@@ -1864,7 +2196,7 @@
     </row>
     <row r="19" spans="2:6" s="26" customFormat="1" ht="23.1" customHeight="1">
       <c r="B19" s="27">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C19" s="31" t="s">
         <v>6</v>
@@ -1875,7 +2207,7 @@
     </row>
     <row r="20" spans="2:6" s="26" customFormat="1" ht="23.1" customHeight="1">
       <c r="B20" s="27">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C20" s="31" t="s">
         <v>6</v>
@@ -1886,7 +2218,7 @@
     </row>
     <row r="21" spans="2:6" s="26" customFormat="1" ht="23.1" customHeight="1">
       <c r="B21" s="27">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C21" s="31" t="s">
         <v>6</v>
@@ -1897,7 +2229,7 @@
     </row>
     <row r="22" spans="2:6" s="26" customFormat="1" ht="23.1" customHeight="1">
       <c r="B22" s="27">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C22" s="31" t="s">
         <v>6</v>
@@ -1908,7 +2240,7 @@
     </row>
     <row r="23" spans="2:6" s="26" customFormat="1" ht="23.1" customHeight="1">
       <c r="B23" s="27">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C23" s="31" t="s">
         <v>6</v>
@@ -1919,7 +2251,7 @@
     </row>
     <row r="24" spans="2:6" s="26" customFormat="1" ht="23.1" customHeight="1">
       <c r="B24" s="27">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C24" s="31" t="s">
         <v>6</v>
@@ -1930,7 +2262,7 @@
     </row>
     <row r="25" spans="2:6" s="26" customFormat="1" ht="23.1" customHeight="1">
       <c r="B25" s="27">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C25" s="31" t="s">
         <v>6</v>
@@ -1941,7 +2273,7 @@
     </row>
     <row r="26" spans="2:6" s="26" customFormat="1" ht="23.1" customHeight="1">
       <c r="B26" s="27">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C26" s="31" t="s">
         <v>6</v>
@@ -1952,7 +2284,7 @@
     </row>
     <row r="27" spans="2:6" s="26" customFormat="1" ht="23.1" customHeight="1">
       <c r="B27" s="27">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C27" s="31" t="s">
         <v>6</v>
@@ -1963,7 +2295,7 @@
     </row>
     <row r="28" spans="2:6" s="26" customFormat="1" ht="23.1" customHeight="1">
       <c r="B28" s="27">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C28" s="31" t="s">
         <v>6</v>
@@ -1973,7 +2305,9 @@
       <c r="F28" s="32"/>
     </row>
     <row r="29" spans="2:6" s="26" customFormat="1" ht="23.1" customHeight="1">
-      <c r="B29" s="27"/>
+      <c r="B29" s="27">
+        <v>22</v>
+      </c>
       <c r="C29" s="31" t="s">
         <v>6</v>
       </c>
@@ -2027,81 +2361,81 @@
       <c r="F34" s="32"/>
     </row>
     <row r="35" spans="2:6" s="15" customFormat="1" ht="23.1" customHeight="1">
-      <c r="B35" s="48"/>
+      <c r="B35" s="47"/>
       <c r="C35" s="33"/>
       <c r="D35" s="30"/>
       <c r="E35" s="30"/>
       <c r="F35" s="34"/>
     </row>
     <row r="36" spans="2:6" s="15" customFormat="1" ht="23.1" customHeight="1">
-      <c r="B36" s="48"/>
+      <c r="B36" s="47"/>
       <c r="C36" s="33"/>
       <c r="D36" s="30"/>
       <c r="E36" s="30"/>
       <c r="F36" s="34"/>
     </row>
     <row r="37" spans="2:6" s="15" customFormat="1" ht="23.1" customHeight="1">
-      <c r="B37" s="48"/>
+      <c r="B37" s="47"/>
       <c r="C37" s="33"/>
       <c r="D37" s="30"/>
       <c r="E37" s="30"/>
       <c r="F37" s="34"/>
     </row>
     <row r="38" spans="2:6" s="15" customFormat="1" ht="23.1" customHeight="1">
-      <c r="B38" s="48"/>
+      <c r="B38" s="47"/>
       <c r="C38" s="33"/>
       <c r="D38" s="30"/>
       <c r="E38" s="30"/>
       <c r="F38" s="34"/>
     </row>
     <row r="39" spans="2:6" s="15" customFormat="1" ht="23.1" customHeight="1">
-      <c r="B39" s="48"/>
+      <c r="B39" s="47"/>
       <c r="C39" s="33"/>
       <c r="D39" s="30"/>
       <c r="E39" s="30"/>
       <c r="F39" s="34"/>
     </row>
     <row r="40" spans="2:6" s="15" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
-      <c r="B40" s="49"/>
+      <c r="B40" s="48"/>
       <c r="C40" s="35"/>
       <c r="D40" s="36"/>
       <c r="E40" s="36"/>
       <c r="F40" s="37"/>
     </row>
     <row r="41" spans="2:6" s="15" customFormat="1" ht="23.1" customHeight="1">
-      <c r="B41" s="50"/>
+      <c r="B41" s="49"/>
       <c r="E41" s="16"/>
     </row>
     <row r="42" spans="2:6" s="15" customFormat="1" ht="23.1" customHeight="1">
-      <c r="B42" s="50"/>
+      <c r="B42" s="49"/>
       <c r="E42" s="16"/>
     </row>
     <row r="43" spans="2:6" s="15" customFormat="1" ht="23.1" customHeight="1">
-      <c r="B43" s="50"/>
+      <c r="B43" s="49"/>
       <c r="E43" s="16"/>
     </row>
     <row r="44" spans="2:6" s="15" customFormat="1" ht="23.1" customHeight="1">
-      <c r="B44" s="50"/>
+      <c r="B44" s="49"/>
       <c r="E44" s="16"/>
     </row>
     <row r="45" spans="2:6" s="15" customFormat="1" ht="23.1" customHeight="1">
-      <c r="B45" s="50"/>
+      <c r="B45" s="49"/>
       <c r="E45" s="16"/>
     </row>
     <row r="46" spans="2:6" s="15" customFormat="1" ht="23.1" customHeight="1">
-      <c r="B46" s="50"/>
+      <c r="B46" s="49"/>
       <c r="E46" s="16"/>
     </row>
     <row r="47" spans="2:6" s="15" customFormat="1" ht="23.1" customHeight="1">
-      <c r="B47" s="50"/>
+      <c r="B47" s="49"/>
       <c r="E47" s="16"/>
     </row>
     <row r="48" spans="2:6" s="15" customFormat="1" ht="23.1" customHeight="1">
-      <c r="B48" s="50"/>
+      <c r="B48" s="49"/>
       <c r="E48" s="16"/>
     </row>
     <row r="49" spans="2:5" s="15" customFormat="1" ht="23.1" customHeight="1">
-      <c r="B49" s="50"/>
+      <c r="B49" s="49"/>
       <c r="E49" s="16"/>
     </row>
     <row r="50" spans="2:5" s="15" customFormat="1" ht="23.1" customHeight="1">
@@ -2115,121 +2449,254 @@
     <mergeCell ref="B2:F2"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
-  <conditionalFormatting sqref="C5:C34 D5 F5:F34">
-    <cfRule type="expression" dxfId="33" priority="51">
+  <conditionalFormatting sqref="C5:C34 F5:F34">
+    <cfRule type="expression" dxfId="72" priority="51">
       <formula>$C5="Done!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="52">
+    <cfRule type="expression" dxfId="71" priority="52">
       <formula>$C5="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="53">
+    <cfRule type="expression" dxfId="70" priority="53">
       <formula>$C5="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="54">
+    <cfRule type="expression" dxfId="69" priority="54">
       <formula>$C5="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="expression" dxfId="29" priority="43">
+    <cfRule type="expression" dxfId="68" priority="43">
+      <formula>$C5="Done!"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="67" priority="44">
+      <formula>$C5="Ongoing"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="66" priority="45">
+      <formula>$C5="Blocked"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="65" priority="46">
+      <formula>$C5="Dropped"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D8">
+    <cfRule type="expression" dxfId="64" priority="35">
       <formula>$C7="Done!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="44">
+    <cfRule type="expression" dxfId="63" priority="36">
       <formula>$C7="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="45">
+    <cfRule type="expression" dxfId="62" priority="37">
       <formula>$C7="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="46">
+    <cfRule type="expression" dxfId="61" priority="38">
       <formula>$C7="Dropped"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D18:D34">
+    <cfRule type="expression" dxfId="60" priority="18">
+      <formula>$C$4="Plannedd"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="59" priority="23">
+      <formula>$C18="Done!"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="58" priority="24">
+      <formula>$C18="Ongoing"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="57" priority="25">
+      <formula>$C18="Blocked"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="56" priority="26">
+      <formula>$C18="Dropped"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B6">
+    <cfRule type="expression" dxfId="55" priority="14">
+      <formula>$C5="Done!"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="54" priority="15">
+      <formula>$C5="Ongoing"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="53" priority="16">
+      <formula>$C5="Blocked"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="52" priority="17">
+      <formula>$C5="Dropped"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8">
+    <cfRule type="expression" dxfId="51" priority="10">
+      <formula>$C7="Done!"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="50" priority="11">
+      <formula>$C7="Ongoing"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="49" priority="12">
+      <formula>$C7="Blocked"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="48" priority="13">
+      <formula>$C7="Dropped"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7">
+    <cfRule type="expression" dxfId="47" priority="6">
+      <formula>$C6="Done!"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="46" priority="7">
+      <formula>$C6="Ongoing"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="45" priority="8">
+      <formula>$C6="Blocked"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="44" priority="9">
+      <formula>$C6="Dropped"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B30:B34">
+    <cfRule type="expression" dxfId="43" priority="1">
+      <formula>$C$4="Plannedd"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="42" priority="2">
+      <formula>$C30="Done!"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="41" priority="3">
+      <formula>$C30="Ongoing"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="40" priority="4">
+      <formula>$C30="Blocked"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="39" priority="5">
+      <formula>$C30="Dropped"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B9:B29 D16:D17">
+    <cfRule type="expression" dxfId="38" priority="60">
+      <formula>$C$4="Plannedd"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="37" priority="61">
+      <formula>$C8="Done!"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="36" priority="62">
+      <formula>$C8="Ongoing"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="35" priority="63">
+      <formula>$C8="Blocked"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="34" priority="64">
+      <formula>$C8="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="expression" dxfId="25" priority="35">
+    <cfRule type="expression" dxfId="33" priority="70">
+      <formula>$C$4="Plannedd"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="32" priority="71">
+      <formula>$C13="Done!"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="31" priority="72">
+      <formula>$C13="Ongoing"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="30" priority="73">
+      <formula>$C13="Blocked"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="29" priority="74">
+      <formula>$C13="Dropped"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D15">
+    <cfRule type="expression" dxfId="28" priority="80">
+      <formula>$C$4="Plannedd"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="27" priority="81">
+      <formula>$C10="Done!"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="26" priority="82">
+      <formula>$C10="Ongoing"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="25" priority="83">
+      <formula>$C10="Blocked"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="24" priority="84">
+      <formula>$C10="Dropped"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D12">
+    <cfRule type="expression" dxfId="23" priority="89">
+      <formula>$C$4="Plannedd"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="22" priority="90">
+      <formula>$C9="Done!"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="21" priority="91">
+      <formula>$C9="Ongoing"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="20" priority="92">
+      <formula>$C9="Blocked"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="19" priority="93">
+      <formula>$C9="Dropped"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D9">
+    <cfRule type="expression" dxfId="18" priority="99">
+      <formula>$C$4="Plannedd"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="17" priority="100">
+      <formula>$C14="Done!"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="101">
+      <formula>$C14="Ongoing"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="15" priority="102">
+      <formula>$C14="Blocked"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="14" priority="103">
+      <formula>$C14="Dropped"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D13">
+    <cfRule type="expression" dxfId="13" priority="108">
       <formula>$C6="Done!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="36">
+    <cfRule type="expression" dxfId="12" priority="109">
       <formula>$C6="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="37">
+    <cfRule type="expression" dxfId="11" priority="110">
       <formula>$C6="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="38">
+    <cfRule type="expression" dxfId="10" priority="111">
       <formula>$C6="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D8:D34">
-    <cfRule type="expression" dxfId="21" priority="18">
+  <conditionalFormatting sqref="D11">
+    <cfRule type="expression" dxfId="9" priority="117">
       <formula>$C$4="Plannedd"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="23">
+    <cfRule type="expression" dxfId="8" priority="118">
+      <formula>$C11="Done!"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="119">
+      <formula>$C11="Ongoing"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="120">
+      <formula>$C11="Blocked"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="121">
+      <formula>$C11="Dropped"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D14 D10">
+    <cfRule type="expression" dxfId="4" priority="122">
+      <formula>$C$4="Plannedd"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="123">
       <formula>$C8="Done!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="24">
+    <cfRule type="expression" dxfId="2" priority="124">
       <formula>$C8="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="25">
+    <cfRule type="expression" dxfId="1" priority="125">
       <formula>$C8="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="26">
-      <formula>$C8="Dropped"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B5">
-    <cfRule type="expression" dxfId="16" priority="14">
-      <formula>$C5="Done!"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="15" priority="15">
-      <formula>$C5="Ongoing"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="14" priority="16">
-      <formula>$C5="Blocked"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="13" priority="17">
-      <formula>$C5="Dropped"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B7">
-    <cfRule type="expression" dxfId="12" priority="10">
-      <formula>$C7="Done!"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="11" priority="11">
-      <formula>$C7="Ongoing"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="12">
-      <formula>$C7="Blocked"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="9" priority="13">
-      <formula>$C7="Dropped"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B6">
-    <cfRule type="expression" dxfId="8" priority="6">
-      <formula>$C6="Done!"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="7" priority="7">
-      <formula>$C6="Ongoing"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="8">
-      <formula>$C6="Blocked"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="5" priority="9">
-      <formula>$C6="Dropped"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B8:B34">
-    <cfRule type="expression" dxfId="4" priority="1">
-      <formula>$C$4="Plannedd"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="3" priority="2">
-      <formula>$C8="Done!"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="3">
-      <formula>$C8="Ongoing"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="4">
-      <formula>$C8="Blocked"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="5">
+    <cfRule type="expression" dxfId="0" priority="126">
       <formula>$C8="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2238,24 +2705,18 @@
   <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
-          <x14:formula1>
-            <xm:f>Dados!$A$2:$A$14</xm:f>
-          </x14:formula1>
-          <xm:sqref>E6:E34</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Dados!$B$2:$B$6</xm:f>
           </x14:formula1>
           <xm:sqref>C5:C34</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Dados!$E$2:$E$4</xm:f>
+            <xm:f>Dados!$A$2:$A$14</xm:f>
           </x14:formula1>
-          <xm:sqref>E5</xm:sqref>
+          <xm:sqref>E6:E15 E16:E34</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2267,7 +2728,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
@@ -2310,11 +2771,11 @@
       <c r="E2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="59" t="s">
+      <c r="H2" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="58"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="18">
@@ -2360,9 +2821,9 @@
       <c r="C5" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="58"/>
-      <c r="I5" s="58"/>
-      <c r="J5" s="58"/>
+      <c r="H5" s="57"/>
+      <c r="I5" s="57"/>
+      <c r="J5" s="57"/>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="18">

</xml_diff>

<commit_message>
BackLog atualizado (Observações e novos requisitos
</commit_message>
<xml_diff>
--- a/documentaçao/ProductBacklog.xlsx
+++ b/documentaçao/ProductBacklog.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="78">
   <si>
     <t>Product BackLog Classified (PBC)</t>
   </si>
@@ -53,33 +53,18 @@
     <t>Planejada</t>
   </si>
   <si>
-    <t>O sistema deverá ter uma dashboard com o uso do hardware de cada processo</t>
-  </si>
-  <si>
     <t xml:space="preserve">Importante </t>
   </si>
   <si>
     <t>O sistema deve monitorar todos os processos ativos</t>
   </si>
   <si>
-    <t>O sistema deve ter uma dashboard para comparação de uso de hardware entre IDEs</t>
-  </si>
-  <si>
     <t>O sistema deverá enviar alertas de sobrecarga do hardware</t>
   </si>
   <si>
-    <t>O sistema deverá fazer uma comaparação de uso de hardware por dia e semana</t>
-  </si>
-  <si>
-    <t>O sistema deverá fazer uma análise isolada da IDE e informar se ainda é prestativa</t>
-  </si>
-  <si>
     <t>O sistema deverá enviar um alerta caso o funcionário esteja a muito tempo sem desenvolver</t>
   </si>
   <si>
-    <t>O sistema deverá gerar relátorios semanalmente</t>
-  </si>
-  <si>
     <t>O sistema deve conter login e senha para acesso usuário</t>
   </si>
   <si>
@@ -89,9 +74,6 @@
     <t>O sistema deverá dectar um sistema com baixo desempenho (sistema legado)</t>
   </si>
   <si>
-    <t>O sistema deverá mandar um alerta caso ele detecte um sistema legado</t>
-  </si>
-  <si>
     <t>Fibonnaci</t>
   </si>
   <si>
@@ -222,6 +204,75 @@
   </si>
   <si>
     <t>EC</t>
+  </si>
+  <si>
+    <t>Persistência de registros a cada 5s</t>
+  </si>
+  <si>
+    <t>Os alertas/notificações devem ser enviados pelo Slack</t>
+  </si>
+  <si>
+    <t>O site institucionar deve ser responsivo</t>
+  </si>
+  <si>
+    <t>O usuário poderá cadastrar os processos que não quer que sejam abertos via Slack</t>
+  </si>
+  <si>
+    <t>O sistema deverá fechar o processo caso ele seja cadastrado no Slack</t>
+  </si>
+  <si>
+    <t>O sistema deverá cadastrar todos os processos em uso pelo dia e hora</t>
+  </si>
+  <si>
+    <t>O sistema deverá comparar IDE's a partir do seu consumo nos processos</t>
+  </si>
+  <si>
+    <t>O sistema deverá fazer uma comaparação de uso de hardware por semana</t>
+  </si>
+  <si>
+    <t>(Funcionalidade)</t>
+  </si>
+  <si>
+    <t>Requisito</t>
+  </si>
+  <si>
+    <t>O sistema deverá fazer uma análise do processo da IDE e informar se está sobrecarregando o sistema</t>
+  </si>
+  <si>
+    <t>*Alterado, análise isolada da.., ...e informar se ainda é prestativa. (Funcionalidade)</t>
+  </si>
+  <si>
+    <t>O sistema deverá mandar um alerta caso ele detecte um sistema legado, via Slack</t>
+  </si>
+  <si>
+    <r>
+      <t>Requisito</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Barlow"/>
+      </rPr>
+      <t>. Mas como fariamos isso. Analise de Processos? Hardware?</t>
+    </r>
+  </si>
+  <si>
+    <t>Requisito. *Alterado, via Slack</t>
+  </si>
+  <si>
+    <t>Requisito (Inovação)</t>
+  </si>
+  <si>
+    <t>O sistema deve ter uma dashboard para comparação de uso de hardware entre IDEs escolhidas pelo gestor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Funcionalidade) *Alterado por dia e semana </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Requisito *Alterado, antes era uma dashboard para cada processo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Requisito </t>
   </si>
 </sst>
 </file>
@@ -231,7 +282,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -323,13 +374,17 @@
     </font>
     <font>
       <u/>
-      <sz val="14"/>
+      <sz val="12"/>
       <name val="Barlow"/>
     </font>
     <font>
-      <u/>
+      <sz val="10"/>
+      <name val="Barlow"/>
+    </font>
+    <font>
       <sz val="12"/>
-      <name val="Barlow"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="14">
@@ -655,7 +710,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -734,10 +789,6 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -821,6 +872,10 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -836,11 +891,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -867,7 +927,113 @@
     <cellStyle name="Hiperlink Visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="73">
+  <dxfs count="86">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFEFB661"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFC8D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFEFB661"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFC8D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FFEFB661"/>
+          <bgColor rgb="FFEFB661"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFC8D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1583,7 +1749,7 @@
         <xdr:cNvPr id="4" name="Imagem 3" descr="Logo SPTECH">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28E092BE-8680-4E85-8060-49F631E5D5E9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{28E092BE-8680-4E85-8060-49F631E5D5E9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1953,8 +2119,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H51"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="23.1" customHeight="1"/>
@@ -1962,9 +2128,9 @@
     <col min="1" max="1" width="3.85546875" style="4" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.140625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="92.140625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="101.5703125" style="4" customWidth="1"/>
     <col min="5" max="5" width="16.28515625" style="14" customWidth="1"/>
-    <col min="6" max="6" width="51.5703125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="69" style="4" customWidth="1"/>
     <col min="7" max="8" width="8.85546875" style="4"/>
     <col min="9" max="9" width="13.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="8.85546875" style="4"/>
@@ -1983,459 +2149,474 @@
     </row>
     <row r="3" spans="2:8" ht="9.9499999999999993" customHeight="1" thickBot="1"/>
     <row r="4" spans="2:8" s="25" customFormat="1" ht="43.5" customHeight="1" thickBot="1">
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="40" t="s">
+      <c r="C4" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="42" t="s">
+      <c r="D4" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="43" t="s">
+      <c r="E4" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="44" t="s">
+      <c r="F4" s="43" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="2:8" s="26" customFormat="1" ht="23.1" customHeight="1">
-      <c r="C5" s="38"/>
-      <c r="F5" s="39"/>
+      <c r="C5" s="37"/>
+      <c r="F5" s="38"/>
     </row>
     <row r="6" spans="2:8" s="26" customFormat="1" ht="23.1" customHeight="1">
-      <c r="B6" s="45">
+      <c r="B6" s="44">
         <v>1</v>
       </c>
-      <c r="C6" s="31" t="s">
+      <c r="C6" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="51" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="29">
+      <c r="D6" s="50" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="28">
         <v>2</v>
       </c>
-      <c r="F6" s="32"/>
+      <c r="F6" s="60" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="7" spans="2:8" s="26" customFormat="1" ht="23.1" customHeight="1">
       <c r="B7" s="27">
         <v>2</v>
       </c>
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="50" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="29">
+      <c r="D7" s="49" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" s="28">
         <v>5</v>
       </c>
-      <c r="F7" s="32"/>
+      <c r="F7" s="33" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="8" spans="2:8" s="26" customFormat="1" ht="23.1" customHeight="1">
-      <c r="B8" s="46">
+      <c r="B8" s="45">
         <v>3</v>
       </c>
-      <c r="C8" s="31" t="s">
+      <c r="C8" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="53" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="29">
+      <c r="D8" s="52" t="s">
+        <v>74</v>
+      </c>
+      <c r="E8" s="28">
         <v>3</v>
       </c>
-      <c r="F8" s="32"/>
+      <c r="F8" s="60" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="9" spans="2:8" s="26" customFormat="1" ht="22.5" customHeight="1">
       <c r="B9" s="27">
         <v>4</v>
       </c>
-      <c r="C9" s="31" t="s">
+      <c r="C9" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="52" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="29">
-        <v>8</v>
-      </c>
-      <c r="F9" s="32"/>
+      <c r="D9" s="59" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9" s="26">
+        <v>5</v>
+      </c>
+      <c r="F9" s="31" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="10" spans="2:8" s="26" customFormat="1" ht="23.1" customHeight="1">
       <c r="B10" s="27">
         <v>3</v>
       </c>
-      <c r="C10" s="31" t="s">
+      <c r="C10" s="30" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="51" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="29">
+        <v>12</v>
+      </c>
+      <c r="E10" s="28">
         <v>8</v>
       </c>
-      <c r="F10" s="32"/>
+      <c r="F10" s="60" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="11" spans="2:8" s="26" customFormat="1" ht="23.1" customHeight="1">
       <c r="B11" s="27">
         <v>4</v>
       </c>
-      <c r="C11" s="31" t="s">
+      <c r="C11" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="51" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="29">
-        <v>3</v>
-      </c>
-      <c r="F11" s="32"/>
+      <c r="D11" s="50" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="28">
+        <v>8</v>
+      </c>
+      <c r="F11" s="60" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="12" spans="2:8" s="26" customFormat="1" ht="23.1" customHeight="1">
       <c r="B12" s="27">
         <v>5</v>
       </c>
-      <c r="C12" s="31" t="s">
+      <c r="C12" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="52" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="29">
-        <v>5</v>
-      </c>
-      <c r="F12" s="32"/>
+      <c r="D12" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="28">
+        <v>3</v>
+      </c>
+      <c r="F12" s="60" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="13" spans="2:8" s="26" customFormat="1" ht="23.1" customHeight="1">
       <c r="B13" s="27">
         <v>6</v>
       </c>
-      <c r="C13" s="31" t="s">
+      <c r="C13" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="52" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="29">
+      <c r="D13" s="51" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" s="28">
         <v>5</v>
       </c>
-      <c r="F13" s="60"/>
+      <c r="F13" s="33" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="14" spans="2:8" s="26" customFormat="1" ht="23.1" customHeight="1">
       <c r="B14" s="27">
         <v>7</v>
       </c>
-      <c r="C14" s="31" t="s">
+      <c r="C14" s="30" t="s">
         <v>6</v>
       </c>
       <c r="D14" s="51" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" s="29">
-        <v>3</v>
-      </c>
-      <c r="F14" s="32"/>
+        <v>8</v>
+      </c>
+      <c r="E14" s="28">
+        <v>5</v>
+      </c>
+      <c r="F14" s="61" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="15" spans="2:8" s="26" customFormat="1" ht="23.1" customHeight="1">
       <c r="B15" s="27">
         <v>8</v>
       </c>
-      <c r="C15" s="31" t="s">
+      <c r="C15" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="51" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="29">
+      <c r="D15" s="50" t="s">
+        <v>68</v>
+      </c>
+      <c r="E15" s="28">
         <v>5</v>
       </c>
-      <c r="F15" s="32"/>
+      <c r="F15" s="62" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="16" spans="2:8" s="26" customFormat="1" ht="23.1" customHeight="1">
       <c r="B16" s="27">
         <v>9</v>
       </c>
-      <c r="C16" s="31" t="s">
+      <c r="C16" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="59" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16" s="29">
+      <c r="D16" s="53" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="28">
         <v>5</v>
       </c>
-      <c r="F16" s="32"/>
+      <c r="F16" s="31" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="17" spans="2:6" s="26" customFormat="1" ht="23.1" customHeight="1">
       <c r="B17" s="27">
         <v>10</v>
       </c>
-      <c r="C17" s="31" t="s">
+      <c r="C17" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="52" t="s">
-        <v>19</v>
-      </c>
-      <c r="E17" s="29">
+      <c r="D17" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="E17" s="28">
         <v>8</v>
       </c>
-      <c r="F17" s="32"/>
+      <c r="F17" s="31" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="18" spans="2:6" s="26" customFormat="1" ht="23.1" customHeight="1">
       <c r="B18" s="27">
         <v>11</v>
       </c>
-      <c r="C18" s="31" t="s">
+      <c r="C18" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="28"/>
-      <c r="E18" s="29"/>
-      <c r="F18" s="32"/>
+      <c r="D18" s="51" t="s">
+        <v>58</v>
+      </c>
+      <c r="E18" s="28">
+        <v>2</v>
+      </c>
+      <c r="F18" s="31" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="19" spans="2:6" s="26" customFormat="1" ht="23.1" customHeight="1">
       <c r="B19" s="27">
         <v>12</v>
       </c>
-      <c r="C19" s="31" t="s">
+      <c r="C19" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="28"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="32"/>
+      <c r="D19" s="51" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" s="28">
+        <v>5</v>
+      </c>
+      <c r="F19" s="31" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="20" spans="2:6" s="26" customFormat="1" ht="23.1" customHeight="1">
       <c r="B20" s="27">
         <v>13</v>
       </c>
-      <c r="C20" s="31" t="s">
+      <c r="C20" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="28"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="32"/>
+      <c r="D20" s="51" t="s">
+        <v>60</v>
+      </c>
+      <c r="E20" s="28">
+        <v>5</v>
+      </c>
+      <c r="F20" s="31" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="21" spans="2:6" s="26" customFormat="1" ht="23.1" customHeight="1">
       <c r="B21" s="27">
         <v>14</v>
       </c>
-      <c r="C21" s="31" t="s">
+      <c r="C21" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="D21" s="28"/>
-      <c r="E21" s="29"/>
-      <c r="F21" s="32"/>
+      <c r="D21" s="51" t="s">
+        <v>61</v>
+      </c>
+      <c r="E21" s="28">
+        <v>8</v>
+      </c>
+      <c r="F21" s="31" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="22" spans="2:6" s="26" customFormat="1" ht="23.1" customHeight="1">
       <c r="B22" s="27">
         <v>15</v>
       </c>
-      <c r="C22" s="31" t="s">
+      <c r="C22" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="28"/>
-      <c r="E22" s="29"/>
-      <c r="F22" s="32"/>
+      <c r="D22" s="51" t="s">
+        <v>62</v>
+      </c>
+      <c r="E22" s="28">
+        <v>8</v>
+      </c>
+      <c r="F22" s="31" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="23" spans="2:6" s="26" customFormat="1" ht="23.1" customHeight="1">
       <c r="B23" s="27">
         <v>16</v>
       </c>
-      <c r="C23" s="31" t="s">
+      <c r="C23" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="D23" s="28"/>
+      <c r="D23" s="29"/>
       <c r="E23" s="29"/>
-      <c r="F23" s="32"/>
+      <c r="F23" s="33"/>
     </row>
     <row r="24" spans="2:6" s="26" customFormat="1" ht="23.1" customHeight="1">
       <c r="B24" s="27">
         <v>17</v>
       </c>
-      <c r="C24" s="31" t="s">
+      <c r="C24" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="D24" s="28"/>
+      <c r="D24" s="29"/>
       <c r="E24" s="29"/>
-      <c r="F24" s="32"/>
+      <c r="F24" s="33"/>
     </row>
     <row r="25" spans="2:6" s="26" customFormat="1" ht="23.1" customHeight="1">
       <c r="B25" s="27">
         <v>18</v>
       </c>
-      <c r="C25" s="31" t="s">
+      <c r="C25" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="D25" s="28"/>
+      <c r="D25" s="29"/>
       <c r="E25" s="29"/>
-      <c r="F25" s="32"/>
+      <c r="F25" s="33"/>
     </row>
     <row r="26" spans="2:6" s="26" customFormat="1" ht="23.1" customHeight="1">
       <c r="B26" s="27">
         <v>19</v>
       </c>
-      <c r="C26" s="31" t="s">
+      <c r="C26" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="D26" s="27"/>
+      <c r="D26" s="29"/>
       <c r="E26" s="29"/>
-      <c r="F26" s="32"/>
-    </row>
-    <row r="27" spans="2:6" s="26" customFormat="1" ht="23.1" customHeight="1">
+      <c r="F26" s="33"/>
+    </row>
+    <row r="27" spans="2:6" s="26" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
       <c r="B27" s="27">
         <v>20</v>
       </c>
-      <c r="C27" s="31" t="s">
+      <c r="C27" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="D27" s="27"/>
-      <c r="E27" s="29"/>
-      <c r="F27" s="32"/>
+      <c r="D27" s="35"/>
+      <c r="E27" s="35"/>
+      <c r="F27" s="36"/>
     </row>
     <row r="28" spans="2:6" s="26" customFormat="1" ht="23.1" customHeight="1">
       <c r="B28" s="27">
         <v>21</v>
       </c>
-      <c r="C28" s="31" t="s">
+      <c r="C28" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="D28" s="27"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="32"/>
     </row>
     <row r="29" spans="2:6" s="26" customFormat="1" ht="23.1" customHeight="1">
       <c r="B29" s="27">
         <v>22</v>
       </c>
-      <c r="C29" s="31" t="s">
+      <c r="C29" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="D29" s="27"/>
-      <c r="E29" s="29"/>
-      <c r="F29" s="32"/>
     </row>
     <row r="30" spans="2:6" s="26" customFormat="1" ht="23.1" customHeight="1">
       <c r="B30" s="27"/>
-      <c r="C30" s="31" t="s">
+      <c r="C30" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="D30" s="27"/>
-      <c r="E30" s="29"/>
-      <c r="F30" s="32"/>
     </row>
     <row r="31" spans="2:6" s="26" customFormat="1" ht="23.1" customHeight="1">
       <c r="B31" s="27"/>
-      <c r="C31" s="31" t="s">
+      <c r="C31" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="D31" s="27"/>
-      <c r="E31" s="29"/>
-      <c r="F31" s="32"/>
     </row>
     <row r="32" spans="2:6" s="26" customFormat="1" ht="23.1" customHeight="1">
       <c r="B32" s="27"/>
-      <c r="C32" s="31" t="s">
+      <c r="C32" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="D32" s="27"/>
-      <c r="E32" s="29"/>
-      <c r="F32" s="32"/>
-    </row>
-    <row r="33" spans="2:6" s="26" customFormat="1" ht="23.1" customHeight="1">
+    </row>
+    <row r="33" spans="2:5" s="26" customFormat="1" ht="23.1" customHeight="1">
       <c r="B33" s="27"/>
-      <c r="C33" s="31" t="s">
+      <c r="C33" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="D33" s="27"/>
-      <c r="E33" s="29"/>
-      <c r="F33" s="32"/>
-    </row>
-    <row r="34" spans="2:6" s="26" customFormat="1" ht="23.1" customHeight="1">
+    </row>
+    <row r="34" spans="2:5" s="26" customFormat="1" ht="23.1" customHeight="1">
       <c r="B34" s="27"/>
-      <c r="C34" s="31" t="s">
+      <c r="C34" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="D34" s="27"/>
-      <c r="E34" s="29"/>
-      <c r="F34" s="32"/>
-    </row>
-    <row r="35" spans="2:6" s="15" customFormat="1" ht="23.1" customHeight="1">
-      <c r="B35" s="47"/>
-      <c r="C35" s="33"/>
-      <c r="D35" s="30"/>
-      <c r="E35" s="30"/>
-      <c r="F35" s="34"/>
-    </row>
-    <row r="36" spans="2:6" s="15" customFormat="1" ht="23.1" customHeight="1">
-      <c r="B36" s="47"/>
-      <c r="C36" s="33"/>
-      <c r="D36" s="30"/>
-      <c r="E36" s="30"/>
-      <c r="F36" s="34"/>
-    </row>
-    <row r="37" spans="2:6" s="15" customFormat="1" ht="23.1" customHeight="1">
-      <c r="B37" s="47"/>
-      <c r="C37" s="33"/>
-      <c r="D37" s="30"/>
-      <c r="E37" s="30"/>
-      <c r="F37" s="34"/>
-    </row>
-    <row r="38" spans="2:6" s="15" customFormat="1" ht="23.1" customHeight="1">
-      <c r="B38" s="47"/>
-      <c r="C38" s="33"/>
-      <c r="D38" s="30"/>
-      <c r="E38" s="30"/>
-      <c r="F38" s="34"/>
-    </row>
-    <row r="39" spans="2:6" s="15" customFormat="1" ht="23.1" customHeight="1">
-      <c r="B39" s="47"/>
-      <c r="C39" s="33"/>
-      <c r="D39" s="30"/>
-      <c r="E39" s="30"/>
-      <c r="F39" s="34"/>
-    </row>
-    <row r="40" spans="2:6" s="15" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
-      <c r="B40" s="48"/>
-      <c r="C40" s="35"/>
-      <c r="D40" s="36"/>
-      <c r="E40" s="36"/>
-      <c r="F40" s="37"/>
-    </row>
-    <row r="41" spans="2:6" s="15" customFormat="1" ht="23.1" customHeight="1">
-      <c r="B41" s="49"/>
+    </row>
+    <row r="35" spans="2:5" s="15" customFormat="1" ht="23.1" customHeight="1">
+      <c r="B35" s="46"/>
+      <c r="C35" s="32"/>
+    </row>
+    <row r="36" spans="2:5" s="15" customFormat="1" ht="23.1" customHeight="1">
+      <c r="B36" s="46"/>
+      <c r="C36" s="32"/>
+    </row>
+    <row r="37" spans="2:5" s="15" customFormat="1" ht="23.1" customHeight="1">
+      <c r="B37" s="46"/>
+      <c r="C37" s="32"/>
+    </row>
+    <row r="38" spans="2:5" s="15" customFormat="1" ht="23.1" customHeight="1">
+      <c r="B38" s="46"/>
+      <c r="C38" s="32"/>
+    </row>
+    <row r="39" spans="2:5" s="15" customFormat="1" ht="23.1" customHeight="1">
+      <c r="B39" s="46"/>
+      <c r="C39" s="32"/>
+    </row>
+    <row r="40" spans="2:5" s="15" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+      <c r="B40" s="47"/>
+      <c r="C40" s="34"/>
+    </row>
+    <row r="41" spans="2:5" s="15" customFormat="1" ht="23.1" customHeight="1">
+      <c r="B41" s="48"/>
       <c r="E41" s="16"/>
     </row>
-    <row r="42" spans="2:6" s="15" customFormat="1" ht="23.1" customHeight="1">
-      <c r="B42" s="49"/>
+    <row r="42" spans="2:5" s="15" customFormat="1" ht="23.1" customHeight="1">
+      <c r="B42" s="48"/>
       <c r="E42" s="16"/>
     </row>
-    <row r="43" spans="2:6" s="15" customFormat="1" ht="23.1" customHeight="1">
-      <c r="B43" s="49"/>
+    <row r="43" spans="2:5" s="15" customFormat="1" ht="23.1" customHeight="1">
+      <c r="B43" s="48"/>
       <c r="E43" s="16"/>
     </row>
-    <row r="44" spans="2:6" s="15" customFormat="1" ht="23.1" customHeight="1">
-      <c r="B44" s="49"/>
+    <row r="44" spans="2:5" s="15" customFormat="1" ht="23.1" customHeight="1">
+      <c r="B44" s="48"/>
       <c r="E44" s="16"/>
     </row>
-    <row r="45" spans="2:6" s="15" customFormat="1" ht="23.1" customHeight="1">
-      <c r="B45" s="49"/>
+    <row r="45" spans="2:5" s="15" customFormat="1" ht="23.1" customHeight="1">
+      <c r="B45" s="48"/>
       <c r="E45" s="16"/>
     </row>
-    <row r="46" spans="2:6" s="15" customFormat="1" ht="23.1" customHeight="1">
-      <c r="B46" s="49"/>
+    <row r="46" spans="2:5" s="15" customFormat="1" ht="23.1" customHeight="1">
+      <c r="B46" s="48"/>
       <c r="E46" s="16"/>
     </row>
-    <row r="47" spans="2:6" s="15" customFormat="1" ht="23.1" customHeight="1">
-      <c r="B47" s="49"/>
+    <row r="47" spans="2:5" s="15" customFormat="1" ht="23.1" customHeight="1">
+      <c r="B47" s="48"/>
       <c r="E47" s="16"/>
     </row>
-    <row r="48" spans="2:6" s="15" customFormat="1" ht="23.1" customHeight="1">
-      <c r="B48" s="49"/>
+    <row r="48" spans="2:5" s="15" customFormat="1" ht="23.1" customHeight="1">
+      <c r="B48" s="48"/>
       <c r="E48" s="16"/>
     </row>
     <row r="49" spans="2:5" s="15" customFormat="1" ht="23.1" customHeight="1">
-      <c r="B49" s="49"/>
+      <c r="B49" s="48"/>
       <c r="E49" s="16"/>
     </row>
     <row r="50" spans="2:5" s="15" customFormat="1" ht="23.1" customHeight="1">
@@ -2449,255 +2630,300 @@
     <mergeCell ref="B2:F2"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
-  <conditionalFormatting sqref="C5:C34 F5:F34">
-    <cfRule type="expression" dxfId="72" priority="51">
+  <conditionalFormatting sqref="C5:C34 F5:F8">
+    <cfRule type="expression" dxfId="85" priority="51">
       <formula>$C5="Done!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="71" priority="52">
+    <cfRule type="expression" dxfId="84" priority="52">
       <formula>$C5="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="53">
+    <cfRule type="expression" dxfId="83" priority="53">
       <formula>$C5="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="54">
+    <cfRule type="expression" dxfId="82" priority="54">
       <formula>$C5="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="expression" dxfId="68" priority="43">
+    <cfRule type="expression" dxfId="81" priority="43">
       <formula>$C5="Done!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="67" priority="44">
+    <cfRule type="expression" dxfId="80" priority="44">
       <formula>$C5="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="45">
+    <cfRule type="expression" dxfId="79" priority="45">
       <formula>$C5="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="65" priority="46">
+    <cfRule type="expression" dxfId="78" priority="46">
       <formula>$C5="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="expression" dxfId="64" priority="35">
+    <cfRule type="expression" dxfId="77" priority="35">
       <formula>$C7="Done!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="36">
+    <cfRule type="expression" dxfId="76" priority="36">
       <formula>$C7="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="37">
+    <cfRule type="expression" dxfId="75" priority="37">
       <formula>$C7="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="38">
+    <cfRule type="expression" dxfId="74" priority="38">
       <formula>$C7="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D18:D34">
-    <cfRule type="expression" dxfId="60" priority="18">
+  <conditionalFormatting sqref="D16:D17">
+    <cfRule type="expression" dxfId="73" priority="18">
       <formula>$C$4="Plannedd"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="59" priority="23">
-      <formula>$C18="Done!"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="58" priority="24">
-      <formula>$C18="Ongoing"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="57" priority="25">
-      <formula>$C18="Blocked"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="56" priority="26">
-      <formula>$C18="Dropped"</formula>
+    <cfRule type="expression" dxfId="72" priority="23">
+      <formula>$C15="Done!"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="71" priority="24">
+      <formula>$C15="Ongoing"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="70" priority="25">
+      <formula>$C15="Blocked"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="69" priority="26">
+      <formula>$C15="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="expression" dxfId="55" priority="14">
+    <cfRule type="expression" dxfId="68" priority="14">
       <formula>$C5="Done!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="15">
+    <cfRule type="expression" dxfId="67" priority="15">
       <formula>$C5="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="53" priority="16">
+    <cfRule type="expression" dxfId="66" priority="16">
       <formula>$C5="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="17">
+    <cfRule type="expression" dxfId="65" priority="17">
       <formula>$C5="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="expression" dxfId="51" priority="10">
+    <cfRule type="expression" dxfId="64" priority="10">
       <formula>$C7="Done!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="11">
+    <cfRule type="expression" dxfId="63" priority="11">
       <formula>$C7="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="12">
+    <cfRule type="expression" dxfId="62" priority="12">
       <formula>$C7="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="13">
+    <cfRule type="expression" dxfId="61" priority="13">
       <formula>$C7="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="expression" dxfId="47" priority="6">
+    <cfRule type="expression" dxfId="60" priority="6">
       <formula>$C6="Done!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="7">
+    <cfRule type="expression" dxfId="59" priority="7">
       <formula>$C6="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="8">
+    <cfRule type="expression" dxfId="58" priority="8">
       <formula>$C6="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="9">
+    <cfRule type="expression" dxfId="57" priority="9">
       <formula>$C6="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B30:B34">
-    <cfRule type="expression" dxfId="43" priority="1">
+    <cfRule type="expression" dxfId="56" priority="1">
       <formula>$C$4="Plannedd"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="2">
+    <cfRule type="expression" dxfId="55" priority="2">
       <formula>$C30="Done!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="3">
+    <cfRule type="expression" dxfId="54" priority="3">
       <formula>$C30="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="4">
+    <cfRule type="expression" dxfId="53" priority="4">
       <formula>$C30="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="5">
+    <cfRule type="expression" dxfId="52" priority="5">
       <formula>$C30="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B9:B29 D16:D17">
-    <cfRule type="expression" dxfId="38" priority="60">
+  <conditionalFormatting sqref="B9:B29">
+    <cfRule type="expression" dxfId="51" priority="60">
       <formula>$C$4="Plannedd"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="61">
+    <cfRule type="expression" dxfId="50" priority="61">
       <formula>$C8="Done!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="62">
+    <cfRule type="expression" dxfId="49" priority="62">
       <formula>$C8="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="63">
+    <cfRule type="expression" dxfId="48" priority="63">
       <formula>$C8="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="64">
+    <cfRule type="expression" dxfId="47" priority="64">
       <formula>$C8="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="expression" dxfId="33" priority="70">
+    <cfRule type="expression" dxfId="46" priority="70">
       <formula>$C$4="Plannedd"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="71">
+    <cfRule type="expression" dxfId="45" priority="71">
       <formula>$C13="Done!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="72">
+    <cfRule type="expression" dxfId="44" priority="72">
       <formula>$C13="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="73">
+    <cfRule type="expression" dxfId="43" priority="73">
       <formula>$C13="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="74">
+    <cfRule type="expression" dxfId="42" priority="74">
       <formula>$C13="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15">
-    <cfRule type="expression" dxfId="28" priority="80">
+    <cfRule type="expression" dxfId="41" priority="80">
       <formula>$C$4="Plannedd"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="81">
+    <cfRule type="expression" dxfId="40" priority="81">
       <formula>$C10="Done!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="82">
+    <cfRule type="expression" dxfId="39" priority="82">
       <formula>$C10="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="83">
+    <cfRule type="expression" dxfId="38" priority="83">
       <formula>$C10="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="84">
+    <cfRule type="expression" dxfId="37" priority="84">
       <formula>$C10="Dropped"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D13">
+    <cfRule type="expression" dxfId="36" priority="89">
+      <formula>$C$4="Plannedd"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="35" priority="90">
+      <formula>$C9="Done!"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="34" priority="91">
+      <formula>$C9="Ongoing"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="33" priority="92">
+      <formula>$C9="Blocked"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="32" priority="93">
+      <formula>$C9="Dropped"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D10">
+    <cfRule type="expression" dxfId="31" priority="99">
+      <formula>$C$4="Plannedd"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="30" priority="100">
+      <formula>$C14="Done!"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="29" priority="101">
+      <formula>$C14="Ongoing"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="28" priority="102">
+      <formula>$C14="Blocked"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="27" priority="103">
+      <formula>$C14="Dropped"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D14">
+    <cfRule type="expression" dxfId="26" priority="108">
+      <formula>$C6="Done!"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="25" priority="109">
+      <formula>$C6="Ongoing"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="24" priority="110">
+      <formula>$C6="Blocked"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="23" priority="111">
+      <formula>$C6="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12">
-    <cfRule type="expression" dxfId="23" priority="89">
+    <cfRule type="expression" dxfId="22" priority="117">
       <formula>$C$4="Plannedd"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="90">
-      <formula>$C9="Done!"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="21" priority="91">
-      <formula>$C9="Ongoing"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="20" priority="92">
-      <formula>$C9="Blocked"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="19" priority="93">
-      <formula>$C9="Dropped"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D9">
-    <cfRule type="expression" dxfId="18" priority="99">
-      <formula>$C$4="Plannedd"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="17" priority="100">
-      <formula>$C14="Done!"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="16" priority="101">
-      <formula>$C14="Ongoing"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="15" priority="102">
-      <formula>$C14="Blocked"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="14" priority="103">
-      <formula>$C14="Dropped"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D13">
-    <cfRule type="expression" dxfId="13" priority="108">
-      <formula>$C6="Done!"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="12" priority="109">
-      <formula>$C6="Ongoing"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="11" priority="110">
-      <formula>$C6="Blocked"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="111">
-      <formula>$C6="Dropped"</formula>
+    <cfRule type="expression" dxfId="21" priority="118">
+      <formula>$C11="Done!"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="20" priority="119">
+      <formula>$C11="Ongoing"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="19" priority="120">
+      <formula>$C11="Blocked"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="121">
+      <formula>$C11="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11">
-    <cfRule type="expression" dxfId="9" priority="117">
+    <cfRule type="expression" dxfId="17" priority="122">
       <formula>$C$4="Plannedd"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="118">
-      <formula>$C11="Done!"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="7" priority="119">
-      <formula>$C11="Ongoing"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="120">
-      <formula>$C11="Blocked"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="5" priority="121">
-      <formula>$C11="Dropped"</formula>
+    <cfRule type="expression" dxfId="16" priority="123">
+      <formula>$C8="Done!"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="15" priority="124">
+      <formula>$C8="Ongoing"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="14" priority="125">
+      <formula>$C8="Blocked"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="126">
+      <formula>$C8="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D14 D10">
-    <cfRule type="expression" dxfId="4" priority="122">
+  <conditionalFormatting sqref="D18:D22">
+    <cfRule type="expression" dxfId="12" priority="132">
       <formula>$C$4="Plannedd"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="123">
-      <formula>$C8="Done!"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="124">
-      <formula>$C8="Ongoing"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="125">
-      <formula>$C8="Blocked"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="126">
-      <formula>$C8="Dropped"</formula>
+    <cfRule type="expression" dxfId="11" priority="133">
+      <formula>$C18="Done!"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="134">
+      <formula>$C18="Ongoing"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="135">
+      <formula>$C18="Blocked"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="136">
+      <formula>$C18="Dropped"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F10:F22">
+    <cfRule type="expression" dxfId="7" priority="141">
+      <formula>$C9="Done!"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="142">
+      <formula>$C9="Ongoing"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="143">
+      <formula>$C9="Blocked"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="144">
+      <formula>$C9="Dropped"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F9">
+    <cfRule type="expression" dxfId="3" priority="145">
+      <formula>$C22="Done!"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="146">
+      <formula>$C22="Ongoing"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="147">
+      <formula>$C22="Blocked"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="148">
+      <formula>$C22="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2716,7 +2942,7 @@
           <x14:formula1>
             <xm:f>Dados!$A$2:$A$14</xm:f>
           </x14:formula1>
-          <xm:sqref>E6:E15 E16:E34</xm:sqref>
+          <xm:sqref>E6:E8 E10:E22</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2746,13 +2972,13 @@
   <sheetData>
     <row r="1" spans="1:11" s="3" customFormat="1" ht="30" customHeight="1">
       <c r="A1" s="22" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>4</v>
@@ -2763,16 +2989,16 @@
         <v>0</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H2" s="58" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="I2" s="58"/>
       <c r="J2" s="58"/>
@@ -2782,13 +3008,13 @@
         <v>0.5</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H3" s="7"/>
       <c r="I3" s="8"/>
@@ -2799,13 +3025,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="H4" s="9"/>
       <c r="I4" s="10"/>
@@ -2816,10 +3042,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="H5" s="57"/>
       <c r="I5" s="57"/>
@@ -2834,7 +3060,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="K6" s="13"/>
     </row>
@@ -2845,7 +3071,7 @@
       </c>
       <c r="B7" s="18"/>
       <c r="C7" s="19" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -2855,7 +3081,7 @@
       </c>
       <c r="B8" s="18"/>
       <c r="C8" s="19" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -2865,7 +3091,7 @@
       </c>
       <c r="B9" s="18"/>
       <c r="C9" s="19" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -2875,7 +3101,7 @@
       </c>
       <c r="B10" s="18"/>
       <c r="C10" s="19" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -2904,105 +3130,105 @@
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="5" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="6"/>
     </row>
     <row r="16" spans="1:11" ht="68.25" customHeight="1">
       <c r="A16" s="24" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="23.25">
       <c r="A17" s="21" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="23.25">
       <c r="A18" s="21" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="23.25">
       <c r="A19" s="21" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="23.25">
       <c r="A20" s="21" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="23.25">
       <c r="A21" s="21" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="23.25">
       <c r="A22" s="21" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="23.25">
       <c r="A23" s="21" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="23.25">
       <c r="A24" s="21" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="23.25">
       <c r="A25" s="21" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="23.25">
       <c r="A26" s="21" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="23.25">
       <c r="A27" s="21" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>